<commit_message>
se cambio la ux
</commit_message>
<xml_diff>
--- a/docs/GANTT APP SELECCION.xlsx
+++ b/docs/GANTT APP SELECCION.xlsx
@@ -22,7 +22,7 @@
     <definedName name="Etapa">OFFSET(Reportes!$N$6,1,0,COUNTA(Reportes!$N$7:$N$107)-COUNTIF(Reportes!$N$7:$N$26,"")+1,1)</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr autoRecover="0" repairLoad="1"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1694,6 +1694,43 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1740,43 +1777,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2048,7 +2048,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2060,7 +2060,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2152,7 +2152,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2164,7 +2164,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6227,17 +6227,17 @@
     </row>
     <row r="3" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="25"/>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
       <c r="L3" s="25"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -6545,8 +6545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DI84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52:C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.28515625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -6597,17 +6597,17 @@
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:113" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="67" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="68"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="81"/>
       <c r="I3" s="35"/>
       <c r="J3" s="35"/>
       <c r="K3" s="35"/>
@@ -6615,17 +6615,17 @@
       <c r="M3" s="45"/>
     </row>
     <row r="4" spans="1:113" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="69">
+      <c r="C4" s="77"/>
+      <c r="D4" s="82">
         <v>45966</v>
       </c>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="70"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="83"/>
       <c r="I4" s="35"/>
       <c r="J4" s="35"/>
       <c r="K4" s="35"/>
@@ -6639,17 +6639,17 @@
     </row>
     <row r="5" spans="1:113" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="57"/>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="71">
+      <c r="C5" s="77"/>
+      <c r="D5" s="84">
         <v>25</v>
       </c>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="72"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="85"/>
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
       <c r="K5" s="35"/>
@@ -6663,18 +6663,18 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:113" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="73">
+      <c r="C6" s="75"/>
+      <c r="D6" s="86">
         <f>IF(D4="","",D4+D5)</f>
         <v>45991</v>
       </c>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="74"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="87"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
       <c r="K6" s="35"/>
@@ -21824,422 +21824,422 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:110" s="85" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="76">
+    <row r="44" spans="2:110" s="69" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="60">
         <f t="shared" si="95"/>
         <v>36</v>
       </c>
-      <c r="C44" s="77" t="s">
+      <c r="C44" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="78">
+      <c r="D44" s="62">
         <v>1</v>
       </c>
-      <c r="E44" s="79">
+      <c r="E44" s="63">
         <v>35</v>
       </c>
-      <c r="F44" s="78" t="s">
+      <c r="F44" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="G44" s="80">
+      <c r="G44" s="64">
         <v>1</v>
       </c>
-      <c r="H44" s="81">
+      <c r="H44" s="65">
         <f t="shared" si="73"/>
         <v>45986</v>
       </c>
-      <c r="I44" s="81">
+      <c r="I44" s="65">
         <f t="shared" si="97"/>
         <v>45986</v>
       </c>
-      <c r="J44" s="82" t="s">
+      <c r="J44" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="K44" s="78" t="s">
+      <c r="K44" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="L44" s="83"/>
-      <c r="M44" s="84" t="str">
+      <c r="L44" s="67"/>
+      <c r="M44" s="68" t="str">
         <f t="shared" si="87"/>
         <v/>
       </c>
-      <c r="O44" s="86" t="str">
+      <c r="O44" s="70" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="P44" s="87" t="str">
+      <c r="P44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="Q44" s="87" t="str">
+      <c r="Q44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="R44" s="87" t="str">
+      <c r="R44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="S44" s="87" t="str">
+      <c r="S44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="T44" s="87" t="str">
+      <c r="T44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="U44" s="87" t="str">
+      <c r="U44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="V44" s="87" t="str">
+      <c r="V44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="W44" s="87" t="str">
+      <c r="W44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="X44" s="87" t="str">
+      <c r="X44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="Y44" s="87" t="str">
+      <c r="Y44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="Z44" s="87" t="str">
+      <c r="Z44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="AA44" s="87" t="str">
+      <c r="AA44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="AB44" s="87" t="str">
+      <c r="AB44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="AC44" s="87" t="str">
+      <c r="AC44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="AD44" s="87" t="str">
+      <c r="AD44" s="71" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="AE44" s="87" t="str">
+      <c r="AE44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AF44" s="87" t="str">
+      <c r="AF44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AG44" s="87" t="str">
+      <c r="AG44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AH44" s="87" t="str">
+      <c r="AH44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AI44" s="87" t="str">
+      <c r="AI44" s="71" t="str">
         <f t="shared" si="96"/>
         <v>x</v>
       </c>
-      <c r="AJ44" s="87" t="str">
+      <c r="AJ44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AK44" s="87" t="str">
+      <c r="AK44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AL44" s="87" t="str">
+      <c r="AL44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AM44" s="87" t="str">
+      <c r="AM44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AN44" s="87" t="str">
+      <c r="AN44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AO44" s="87" t="str">
+      <c r="AO44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AP44" s="87" t="str">
+      <c r="AP44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AQ44" s="87" t="str">
+      <c r="AQ44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AR44" s="87" t="str">
+      <c r="AR44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AS44" s="87" t="str">
+      <c r="AS44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AT44" s="87" t="str">
+      <c r="AT44" s="71" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="AU44" s="87" t="str">
+      <c r="AU44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="AV44" s="87" t="str">
+      <c r="AV44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="AW44" s="87" t="str">
+      <c r="AW44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="AX44" s="87" t="str">
+      <c r="AX44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="AY44" s="87" t="str">
+      <c r="AY44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="AZ44" s="87" t="str">
+      <c r="AZ44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="BA44" s="87" t="str">
+      <c r="BA44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="BB44" s="87" t="str">
+      <c r="BB44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="BC44" s="87" t="str">
+      <c r="BC44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="BD44" s="87" t="str">
+      <c r="BD44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="BE44" s="87" t="str">
+      <c r="BE44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="BF44" s="87" t="str">
+      <c r="BF44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="BG44" s="87" t="str">
+      <c r="BG44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="BH44" s="87" t="str">
+      <c r="BH44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="BI44" s="87" t="str">
+      <c r="BI44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="BJ44" s="87" t="str">
+      <c r="BJ44" s="71" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="BK44" s="87" t="str">
+      <c r="BK44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BL44" s="87" t="str">
+      <c r="BL44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BM44" s="87" t="str">
+      <c r="BM44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BN44" s="87" t="str">
+      <c r="BN44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BO44" s="87" t="str">
+      <c r="BO44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BP44" s="87" t="str">
+      <c r="BP44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BQ44" s="87" t="str">
+      <c r="BQ44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BR44" s="87" t="str">
+      <c r="BR44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BS44" s="87" t="str">
+      <c r="BS44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BT44" s="87" t="str">
+      <c r="BT44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BU44" s="87" t="str">
+      <c r="BU44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BV44" s="87" t="str">
+      <c r="BV44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BW44" s="87" t="str">
+      <c r="BW44" s="71" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="BX44" s="87" t="str">
+      <c r="BX44" s="71" t="str">
         <f t="shared" si="88"/>
         <v/>
       </c>
-      <c r="BY44" s="87" t="str">
+      <c r="BY44" s="71" t="str">
         <f t="shared" si="88"/>
         <v/>
       </c>
-      <c r="BZ44" s="87" t="str">
+      <c r="BZ44" s="71" t="str">
         <f t="shared" si="88"/>
         <v/>
       </c>
-      <c r="CA44" s="87" t="str">
+      <c r="CA44" s="71" t="str">
         <f t="shared" si="88"/>
         <v/>
       </c>
-      <c r="CB44" s="87" t="str">
+      <c r="CB44" s="71" t="str">
         <f t="shared" si="88"/>
         <v/>
       </c>
-      <c r="CC44" s="87" t="str">
+      <c r="CC44" s="71" t="str">
         <f t="shared" si="88"/>
         <v/>
       </c>
-      <c r="CD44" s="87" t="str">
+      <c r="CD44" s="71" t="str">
         <f t="shared" si="88"/>
         <v/>
       </c>
-      <c r="CE44" s="87" t="str">
+      <c r="CE44" s="71" t="str">
         <f t="shared" si="88"/>
         <v/>
       </c>
-      <c r="CF44" s="87" t="str">
+      <c r="CF44" s="71" t="str">
         <f t="shared" si="88"/>
         <v/>
       </c>
-      <c r="CG44" s="87" t="str">
+      <c r="CG44" s="71" t="str">
         <f t="shared" si="88"/>
         <v/>
       </c>
-      <c r="CH44" s="87" t="str">
+      <c r="CH44" s="71" t="str">
         <f t="shared" si="88"/>
         <v/>
       </c>
-      <c r="CI44" s="87" t="str">
+      <c r="CI44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CJ44" s="87" t="str">
+      <c r="CJ44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CK44" s="87" t="str">
+      <c r="CK44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CL44" s="87" t="str">
+      <c r="CL44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CM44" s="87" t="str">
+      <c r="CM44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CN44" s="87" t="str">
+      <c r="CN44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CO44" s="87" t="str">
+      <c r="CO44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CP44" s="87" t="str">
+      <c r="CP44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CQ44" s="87" t="str">
+      <c r="CQ44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CR44" s="87" t="str">
+      <c r="CR44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CS44" s="87" t="str">
+      <c r="CS44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CT44" s="87" t="str">
+      <c r="CT44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CU44" s="87" t="str">
+      <c r="CU44" s="71" t="str">
         <f t="shared" si="89"/>
         <v/>
       </c>
-      <c r="CV44" s="87" t="str">
+      <c r="CV44" s="71" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="CW44" s="87" t="str">
+      <c r="CW44" s="71" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="CX44" s="87" t="str">
+      <c r="CX44" s="71" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="CY44" s="87" t="str">
+      <c r="CY44" s="71" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="CZ44" s="87" t="str">
+      <c r="CZ44" s="71" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="DA44" s="87" t="str">
+      <c r="DA44" s="71" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="DB44" s="87" t="str">
+      <c r="DB44" s="71" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="DC44" s="87" t="str">
+      <c r="DC44" s="71" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="DE44" s="88">
+      <c r="DE44" s="72">
         <f t="shared" si="90"/>
         <v>0</v>
       </c>
-      <c r="DF44" s="88">
+      <c r="DF44" s="72">
         <f t="shared" si="91"/>
         <v>0</v>
       </c>
@@ -30505,7 +30505,7 @@
       </c>
       <c r="C3" s="9">
         <f ca="1">TODAY()</f>
-        <v>45986</v>
+        <v>45990</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
@@ -30523,7 +30523,7 @@
       </c>
       <c r="C5" s="19">
         <f ca="1">IF('Información del proyecto'!D4="","",C3-'Información del proyecto'!D4)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -30532,7 +30532,7 @@
       </c>
       <c r="C6" s="19">
         <f ca="1">IF('Información del proyecto'!D4="","",C4-C5)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N6" s="18" t="s">
         <v>17</v>
@@ -30828,10 +30828,10 @@
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" s="4"/>
-      <c r="F24" s="75" t="s">
+      <c r="F24" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="75"/>
+      <c r="G24" s="88"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>

</xml_diff>

<commit_message>
aplicando mejoras en mensajes de error
</commit_message>
<xml_diff>
--- a/docs/GANTT APP SELECCION.xlsx
+++ b/docs/GANTT APP SELECCION.xlsx
@@ -2048,7 +2048,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2060,7 +2060,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2152,7 +2152,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2164,7 +2164,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6545,8 +6545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DI84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52:C53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.28515625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -22262,15 +22262,15 @@
         <v>60</v>
       </c>
       <c r="G45" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H45" s="29">
         <f t="shared" si="73"/>
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="I45" s="29">
         <f t="shared" si="97"/>
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="J45" s="58" t="s">
         <v>127</v>
@@ -22369,11 +22369,11 @@
       </c>
       <c r="AJ45" s="17" t="str">
         <f t="shared" si="96"/>
-        <v>x</v>
+        <v/>
       </c>
       <c r="AK45" s="17" t="str">
         <f t="shared" si="96"/>
-        <v/>
+        <v>x</v>
       </c>
       <c r="AL45" s="17" t="str">
         <f t="shared" si="96"/>
@@ -22686,11 +22686,11 @@
       </c>
       <c r="H46" s="29">
         <f t="shared" si="73"/>
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="I46" s="29">
         <f t="shared" si="97"/>
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="J46" s="58" t="s">
         <v>127</v>
@@ -22793,11 +22793,11 @@
       </c>
       <c r="AK46" s="17" t="str">
         <f t="shared" si="96"/>
-        <v>x</v>
+        <v/>
       </c>
       <c r="AL46" s="17" t="str">
         <f t="shared" si="96"/>
-        <v/>
+        <v>x</v>
       </c>
       <c r="AM46" s="17" t="str">
         <f t="shared" si="96"/>
@@ -23106,11 +23106,11 @@
       </c>
       <c r="H47" s="29">
         <f t="shared" si="73"/>
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="I47" s="29">
         <f t="shared" si="97"/>
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="J47" s="58" t="s">
         <v>127</v>
@@ -23217,11 +23217,11 @@
       </c>
       <c r="AL47" s="17" t="str">
         <f t="shared" si="96"/>
-        <v>x</v>
+        <v/>
       </c>
       <c r="AM47" s="17" t="str">
         <f t="shared" si="96"/>
-        <v/>
+        <v>x</v>
       </c>
       <c r="AN47" s="17" t="str">
         <f t="shared" si="96"/>
@@ -23526,11 +23526,11 @@
       </c>
       <c r="H48" s="29">
         <f t="shared" si="73"/>
-        <v>45990</v>
+        <v>45991</v>
       </c>
       <c r="I48" s="29">
         <f t="shared" ref="I48:I61" si="104">IF(H48="","",H48+D48-1)</f>
-        <v>45990</v>
+        <v>45991</v>
       </c>
       <c r="J48" s="58" t="s">
         <v>127</v>
@@ -23641,11 +23641,11 @@
       </c>
       <c r="AM48" s="17" t="str">
         <f t="shared" si="96"/>
-        <v>x</v>
+        <v/>
       </c>
       <c r="AN48" s="17" t="str">
         <f t="shared" si="96"/>
-        <v/>
+        <v>x</v>
       </c>
       <c r="AO48" s="17" t="str">
         <f t="shared" si="96"/>
@@ -23946,11 +23946,11 @@
       </c>
       <c r="H49" s="29">
         <f t="shared" si="73"/>
-        <v>45991</v>
+        <v>45992</v>
       </c>
       <c r="I49" s="29">
         <f t="shared" si="104"/>
-        <v>45991</v>
+        <v>45992</v>
       </c>
       <c r="J49" s="58" t="s">
         <v>127</v>
@@ -24065,11 +24065,11 @@
       </c>
       <c r="AN49" s="17" t="str">
         <f t="shared" si="96"/>
-        <v>x</v>
+        <v/>
       </c>
       <c r="AO49" s="17" t="str">
         <f t="shared" si="96"/>
-        <v/>
+        <v>x</v>
       </c>
       <c r="AP49" s="17" t="str">
         <f t="shared" si="96"/>
@@ -24366,11 +24366,11 @@
       </c>
       <c r="H50" s="29">
         <f t="shared" si="73"/>
-        <v>45992</v>
+        <v>45993</v>
       </c>
       <c r="I50" s="29">
         <f t="shared" si="104"/>
-        <v>45992</v>
+        <v>45993</v>
       </c>
       <c r="J50" s="58" t="s">
         <v>127</v>
@@ -24489,11 +24489,11 @@
       </c>
       <c r="AO50" s="17" t="str">
         <f t="shared" si="96"/>
-        <v>x</v>
+        <v/>
       </c>
       <c r="AP50" s="17" t="str">
         <f t="shared" si="96"/>
-        <v/>
+        <v>x</v>
       </c>
       <c r="AQ50" s="17" t="str">
         <f t="shared" si="96"/>
@@ -30505,7 +30505,7 @@
       </c>
       <c r="C3" s="9">
         <f ca="1">TODAY()</f>
-        <v>45990</v>
+        <v>45992</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
@@ -30523,7 +30523,7 @@
       </c>
       <c r="C5" s="19">
         <f ca="1">IF('Información del proyecto'!D4="","",C3-'Información del proyecto'!D4)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -30532,7 +30532,7 @@
       </c>
       <c r="C6" s="19">
         <f ca="1">IF('Información del proyecto'!D4="","",C4-C5)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="N6" s="18" t="s">
         <v>17</v>

</xml_diff>